<commit_message>
Importar usuarios con validaciones y encabezados
</commit_message>
<xml_diff>
--- a/public/datosExporImport/usersImportValidate-CE.xlsx
+++ b/public/datosExporImport/usersImportValidate-CE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="119">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">updated_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario Nuevo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usuarioNuevo@tmp.com</t>
   </si>
   <si>
     <t xml:space="preserve">Prof. Lance Beer IV</t>
@@ -468,10 +474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -480,7 +486,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
@@ -511,10 +517,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>4316052</v>
+        <v>1234567</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>7</v>
@@ -525,42 +531,36 @@
       <c r="E2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>4671951</v>
+        <v>4316052</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>6895530</v>
+        <v>4671951</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>13</v>
@@ -572,41 +572,41 @@
         <v>123456</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>5209040</v>
+        <v>6895530</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5727963</v>
+        <v>5209040</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>18</v>
@@ -618,18 +618,18 @@
         <v>123456</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>8253155</v>
+        <v>5727963</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>20</v>
@@ -641,18 +641,18 @@
         <v>123456</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>4378410</v>
+        <v>8253155</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>22</v>
@@ -664,18 +664,18 @@
         <v>123456</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>6656012</v>
+        <v>4378410</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>24</v>
@@ -687,18 +687,18 @@
         <v>123456</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>5671668</v>
+        <v>6656012</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>26</v>
@@ -710,18 +710,18 @@
         <v>123456</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>8213789</v>
+        <v>5671668</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>28</v>
@@ -733,18 +733,18 @@
         <v>123456</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>7020000</v>
+        <v>8213789</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>30</v>
@@ -756,18 +756,18 @@
         <v>123456</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>7661089</v>
+        <v>7020000</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>32</v>
@@ -779,18 +779,18 @@
         <v>123456</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>6540052</v>
+        <v>7661089</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>34</v>
@@ -802,18 +802,18 @@
         <v>123456</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>4285793</v>
+        <v>6540052</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>36</v>
@@ -825,18 +825,18 @@
         <v>123456</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>5341032</v>
+        <v>4285793</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>38</v>
@@ -848,18 +848,18 @@
         <v>123456</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>4806198</v>
+        <v>5341032</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>40</v>
@@ -871,64 +871,64 @@
         <v>123456</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>4806198</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>3461352</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>4376320</v>
+        <v>3461352</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="E19" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>8163947</v>
+        <v>4376320</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>48</v>
@@ -940,18 +940,18 @@
         <v>123456</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>4178979</v>
+        <v>8163947</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>50</v>
@@ -963,18 +963,18 @@
         <v>123456</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>4574089</v>
+        <v>4178979</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>52</v>
@@ -986,41 +986,41 @@
         <v>123456</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>4121410</v>
+        <v>4574089</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>3316537</v>
+        <v>4121410</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>57</v>
@@ -1032,18 +1032,18 @@
         <v>123456</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>8690285</v>
+        <v>3316537</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1055,18 +1055,18 @@
         <v>123456</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>6337847</v>
+        <v>8690285</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>61</v>
@@ -1078,18 +1078,18 @@
         <v>123456</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>6671758</v>
+        <v>6337847</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>63</v>
@@ -1101,18 +1101,18 @@
         <v>123456</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>7147588</v>
+        <v>6671758</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>65</v>
@@ -1124,18 +1124,18 @@
         <v>123456</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>4371224</v>
+        <v>7147588</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>67</v>
@@ -1147,41 +1147,41 @@
         <v>123456</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>3201337</v>
+        <v>4371224</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="E30" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>4018149</v>
+        <v>3201337</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>72</v>
@@ -1193,18 +1193,18 @@
         <v>123456</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>8449736</v>
+        <v>4018149</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>74</v>
@@ -1216,18 +1216,18 @@
         <v>123456</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>8993476</v>
+        <v>8449736</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>76</v>
@@ -1239,18 +1239,18 @@
         <v>123456</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>5040403</v>
+        <v>8993476</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>78</v>
@@ -1262,18 +1262,18 @@
         <v>123456</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>3071209</v>
+        <v>5040403</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>80</v>
@@ -1285,18 +1285,18 @@
         <v>123456</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>3634460</v>
+        <v>3071209</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>82</v>
@@ -1308,18 +1308,18 @@
         <v>123456</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>6514566</v>
+        <v>3634460</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>84</v>
@@ -1331,18 +1331,18 @@
         <v>123456</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>4084374</v>
+        <v>6514566</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>86</v>
@@ -1354,64 +1354,64 @@
         <v>123456</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>5595122</v>
+        <v>4084374</v>
       </c>
       <c r="C39" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="E39" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>5069296</v>
+        <v>5595122</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="E40" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>8503692</v>
+        <v>5069296</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>94</v>
@@ -1423,18 +1423,18 @@
         <v>123456</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>7157864</v>
+        <v>8503692</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>96</v>
@@ -1446,18 +1446,18 @@
         <v>123456</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>7047089</v>
+        <v>7157864</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>98</v>
@@ -1469,18 +1469,18 @@
         <v>123456</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>8913426</v>
+        <v>7047089</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>100</v>
@@ -1492,18 +1492,18 @@
         <v>123456</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>3793373</v>
+        <v>8913426</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>102</v>
@@ -1515,18 +1515,18 @@
         <v>123456</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>4058255</v>
+        <v>3793373</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>104</v>
@@ -1538,18 +1538,18 @@
         <v>123456</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>5962016</v>
+        <v>4058255</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>106</v>
@@ -1561,18 +1561,18 @@
         <v>123456</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>4449879</v>
+        <v>5962016</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>108</v>
@@ -1584,18 +1584,18 @@
         <v>123456</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>3426506</v>
+        <v>4449879</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>110</v>
@@ -1607,18 +1607,18 @@
         <v>123456</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>8188220</v>
+        <v>3426506</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>112</v>
@@ -1630,18 +1630,18 @@
         <v>123456</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>6641779</v>
+        <v>8188220</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>114</v>
@@ -1653,10 +1653,33 @@
         <v>123456</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G51" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>6641779</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>116</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>